<commit_message>
Kind of got the 3d model working, updated parts
</commit_message>
<xml_diff>
--- a/Plans/Parts.xlsx
+++ b/Plans/Parts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikey\OneDrive\Documents\GitHub\MyResume\argon-dashboard-django\Plans\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grabinski.ma\Documents\GitHub\argon-dashboard-django\Plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB35161-8A97-4D97-9DB7-FA3EF194975A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939DA440-844B-4B9C-A283-72D6E53E4AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35640" yWindow="3285" windowWidth="19920" windowHeight="12330" xr2:uid="{AF8C979F-4DE1-4006-B607-399B4980CA4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AF8C979F-4DE1-4006-B607-399B4980CA4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>Material</t>
   </si>
@@ -147,6 +145,63 @@
   </si>
   <si>
     <t>Masonite 36-in x 80-in x 4-9/16-in Steel Left-Hand Inswing Primed Prehung Front Door with Brickmould Insulating Core</t>
+  </si>
+  <si>
+    <t>Example:</t>
+  </si>
+  <si>
+    <t>20' by 60'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rafters </t>
+  </si>
+  <si>
+    <t>joist</t>
+  </si>
+  <si>
+    <t>studs</t>
+  </si>
+  <si>
+    <t>feet of plate</t>
+  </si>
+  <si>
+    <t>roof 1264.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roof osb </t>
+  </si>
+  <si>
+    <t>siding osb</t>
+  </si>
+  <si>
+    <t>20' by 60' 2 stories 2,400sqft</t>
+  </si>
+  <si>
+    <t>insluation 2353</t>
+  </si>
+  <si>
+    <t>insluation 3440.8</t>
+  </si>
+  <si>
+    <t>wiring feet</t>
+  </si>
+  <si>
+    <t>outlets</t>
+  </si>
+  <si>
+    <t>Drywall</t>
+  </si>
+  <si>
+    <t>units/feet</t>
+  </si>
+  <si>
+    <t>vinyl siding</t>
+  </si>
+  <si>
+    <t>shingles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flooring </t>
   </si>
 </sst>
 </file>
@@ -224,9 +279,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -264,7 +319,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -370,7 +425,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -512,7 +567,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -522,7 +577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52891224-9C48-4B1B-BFA1-82F3ADF40343}">
   <dimension ref="A1:N171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -533,7 +588,8 @@
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="66.5703125" customWidth="1"/>
+    <col min="8" max="8" width="40.140625" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -614,14 +670,14 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E5">
         <v>7.18</v>
       </c>
       <c r="F5">
         <f t="shared" ref="F5:F16" si="0">D5*E5</f>
-        <v>0</v>
+        <v>1436</v>
       </c>
       <c r="N5" t="s">
         <v>9</v>
@@ -701,14 +757,14 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E9">
         <v>15.98</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>639.20000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -722,14 +778,14 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E10">
         <v>26.5</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>901</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -743,14 +799,20 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E11">
         <v>18.22</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1366.5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -764,14 +826,20 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E12">
         <v>3.78</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>37.799999999999997</v>
+      </c>
+      <c r="K12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -794,6 +862,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J13" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13">
+        <v>46</v>
+      </c>
+      <c r="N13" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -806,14 +883,20 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E14">
         <v>59.33</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2729.18</v>
+      </c>
+      <c r="J14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -827,14 +910,20 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E15">
         <v>1.86</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>186</v>
+      </c>
+      <c r="J15" t="s">
+        <v>41</v>
+      </c>
+      <c r="K15">
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -857,8 +946,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -869,17 +964,23 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <v>118</v>
       </c>
       <c r="F17">
         <f>D17*E17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="J17" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -899,8 +1000,14 @@
         <f t="shared" ref="F18:F29" si="1">D18*E18</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>45</v>
+      </c>
+      <c r="K18">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -920,8 +1027,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>49</v>
+      </c>
+      <c r="K19">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -932,17 +1045,23 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E20">
         <v>9.9700000000000006</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1096.7</v>
+      </c>
+      <c r="J20" t="s">
+        <v>50</v>
+      </c>
+      <c r="K20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -962,8 +1081,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>51</v>
+      </c>
+      <c r="K21">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -974,17 +1099,23 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>199</v>
       </c>
       <c r="F22">
         <f>D22*E22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="J22" t="s">
+        <v>53</v>
+      </c>
+      <c r="K22">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1004,8 +1135,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K23">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1025,8 +1162,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>55</v>
+      </c>
+      <c r="K24">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1037,17 +1180,17 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E25">
         <v>40.619999999999997</v>
       </c>
       <c r="F25">
         <f>D25*E25</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1462.32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1068,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1088,8 +1231,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>37</v>
+      </c>
+      <c r="K27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1100,17 +1249,17 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E28">
         <v>77</v>
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3542</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1121,17 +1270,26 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E29">
         <v>66</v>
       </c>
       <c r="F29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="J29" t="s">
+        <v>39</v>
+      </c>
+      <c r="K29">
+        <v>46</v>
+      </c>
+      <c r="M29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1142,17 +1300,26 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E30">
         <v>152.15</v>
       </c>
       <c r="F30">
         <f t="shared" ref="F30:F33" si="2">D30*E30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2282.25</v>
+      </c>
+      <c r="J30" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30">
+        <v>92</v>
+      </c>
+      <c r="M30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1163,17 +1330,23 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E31">
         <v>285</v>
       </c>
       <c r="F31">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>570</v>
+      </c>
+      <c r="J31" t="s">
+        <v>41</v>
+      </c>
+      <c r="K31">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <v>0</v>
       </c>
@@ -1190,8 +1363,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>42</v>
+      </c>
+      <c r="K32">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>0</v>
       </c>
@@ -1208,8 +1387,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>44</v>
+      </c>
+      <c r="K33">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>0</v>
       </c>
@@ -1226,8 +1411,14 @@
         <f t="shared" ref="F34:F48" si="3">D34*E34</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>45</v>
+      </c>
+      <c r="K34">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>0</v>
       </c>
@@ -1245,7 +1436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>0</v>
       </c>
@@ -1263,7 +1454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>0</v>
       </c>
@@ -1281,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>0</v>
       </c>
@@ -1299,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>0</v>
       </c>
@@ -1317,7 +1508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <v>0</v>
       </c>
@@ -1335,7 +1526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <v>0</v>
       </c>
@@ -1353,7 +1544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <v>0</v>
       </c>
@@ -1371,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
         <v>0</v>
       </c>
@@ -1389,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
         <v>0</v>
       </c>
@@ -1407,7 +1598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="1">
         <v>0</v>
       </c>
@@ -1425,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="1">
         <v>0</v>
       </c>
@@ -1440,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
         <v>0</v>
       </c>
@@ -1452,7 +1643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
         <v>0</v>
       </c>
@@ -1469,7 +1660,7 @@
       <c r="C49" s="1"/>
       <c r="F49">
         <f>SUM(F3:F48)</f>
-        <v>0</v>
+        <v>16829.95</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>